<commit_message>
Updated to V0.3 ProIDE.ino
</commit_message>
<xml_diff>
--- a/PHP/Fehlermeldung Pseminar.xlsx
+++ b/PHP/Fehlermeldung Pseminar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon-Luis\Desktop\Schule\P-Seminar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonah\Documents\Arduino\Mensa\Master\MensaProject\PHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF2692C-F40C-4357-A258-A60057716AC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAA9860-26DE-42A7-8321-A2342928C43C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15645" yWindow="7620" windowWidth="21600" windowHeight="11385" xr2:uid="{85A6A073-1C5D-4906-927E-CC4304BE3713}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{85A6A073-1C5D-4906-927E-CC4304BE3713}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Doppelverwendung innherhalb 3h</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Karte nicht im gültigen Datum</t>
+  </si>
+  <si>
+    <t>Karte an diesem Wochentag ungültig</t>
+  </si>
+  <si>
+    <t>Ihre Karten wurde innerhalb 3 Stunden bereits verwendet</t>
+  </si>
+  <si>
+    <t>Ihre Karten ID ist nicht bekannt</t>
+  </si>
+  <si>
+    <t>Karte abglaufen</t>
   </si>
 </sst>
 </file>
@@ -409,7 +421,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,6 +448,9 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -444,6 +459,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -452,6 +470,9 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -459,6 +480,9 @@
       </c>
       <c r="B5" t="s">
         <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>